<commit_message>
Simplified workbook layout for buildFromWorkbook
</commit_message>
<xml_diff>
--- a/inst/models/SEIR.xlsx
+++ b/inst/models/SEIR.xlsx
@@ -5,13 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="vars" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="pars" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="funs" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="eqns" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="declarations" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="equations" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +21,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+  <si>
+    <t xml:space="preserve">type</t>
+  </si>
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -37,6 +38,9 @@
     <t xml:space="preserve">default</t>
   </si>
   <si>
+    <t xml:space="preserve">variable</t>
+  </si>
+  <si>
     <t xml:space="preserve">S</t>
   </si>
   <si>
@@ -64,6 +68,9 @@
     <t xml:space="preserve">recovered, immune</t>
   </si>
   <si>
+    <t xml:space="preserve">parameter</t>
+  </si>
+  <si>
     <t xml:space="preserve">t</t>
   </si>
   <si>
@@ -83,12 +90,6 @@
   </si>
   <si>
     <t xml:space="preserve">recovery rate constant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dummy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NA</t>
   </si>
   <si>
     <t xml:space="preserve">rate</t>
@@ -304,15 +305,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -328,61 +329,127 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
+      <c r="A2" s="0" t="s">
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>80000000</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="3" t="n">
-        <v>80000000</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>800000</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="3" t="n">
-        <v>800000</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>
@@ -401,145 +468,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="25.98"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>0.4</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.39"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:H4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="7.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="8.06"/>
@@ -549,42 +484,42 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>-1</v>
@@ -601,16 +536,16 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>0</v>
@@ -627,16 +562,16 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>0</v>

</xml_diff>